<commit_message>
Added 3D models for footprints
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -40,9 +40,6 @@
     <t>Assembly</t>
   </si>
   <si>
-    <t>649-220316-H041B01LF</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -56,6 +53,9 @@
   </si>
   <si>
     <t>R_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>712-CONSMA020.062-G</t>
   </si>
   <si>
     <t>Hardware</t>
@@ -233,7 +233,7 @@
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
       <protection locked="1" hidden="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
       <protection locked="1" hidden="0"/>
     </xf>
@@ -270,7 +270,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G45" sqref="G45"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="12.75"/>
@@ -799,8 +799,10 @@
           <t>Screw_Terminal_01x04</t>
         </is>
       </c>
-      <c r="E15" s="11" t="s">
-        <v>6</v>
+      <c r="E15" s="11" t="inlineStr">
+        <is>
+          <t>649-220316-H041B01LF</t>
+        </is>
       </c>
       <c r="F15">
         <v>0.89000000000000001</v>
@@ -973,7 +975,7 @@
         </is>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G20">
         <f>C20*F20</f>
@@ -995,18 +997,18 @@
         </is>
       </c>
       <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>3.5u</t>
+        </is>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>3.5u</t>
-        </is>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="F21">
         <v>3.1099999999999999</v>
@@ -1016,7 +1018,7 @@
         <v>3.1099999999999999</v>
       </c>
       <c r="H21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I21" t="s">
         <v>1</v>
@@ -1029,18 +1031,18 @@
         </is>
       </c>
       <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>594n</t>
+        </is>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>594n</t>
-        </is>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="F22">
         <v>3.1099999999999999</v>
@@ -1050,7 +1052,7 @@
         <v>3.1099999999999999</v>
       </c>
       <c r="H22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I22" t="s">
         <v>1</v>
@@ -1168,7 +1170,7 @@
         </is>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -1199,7 +1201,7 @@
         </is>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1232,7 +1234,7 @@
         </is>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -1265,7 +1267,7 @@
         </is>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -1308,17 +1310,15 @@
           <t>Conn_Coaxial</t>
         </is>
       </c>
-      <c r="E30" s="19" t="inlineStr">
-        <is>
-          <t>960-EMPCB.SMAFSTJCHT</t>
-        </is>
+      <c r="E30" s="19" t="s">
+        <v>11</v>
       </c>
       <c r="F30">
-        <v>2.98</v>
+        <v>3.9300000000000002</v>
       </c>
       <c r="G30">
         <f>C30*F30</f>
-        <v>2.98</v>
+        <v>3.9300000000000002</v>
       </c>
       <c r="I30" t="s">
         <v>1</v>
@@ -1344,7 +1344,7 @@
         </is>
       </c>
       <c r="E31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G31">
         <f>C31*F31</f>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="G44">
         <f>SUM(G2:G43)</f>
-        <v>136.02500000000001</v>
+        <v>136.97499999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>